<commit_message>
funcion de calculo de DI generado
</commit_message>
<xml_diff>
--- a/Resultados/P_18.xlsx
+++ b/Resultados/P_18.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2" uniqueCount="1">
   <si>
     <t>P</t>
   </si>
@@ -77,182 +77,182 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>2.1372761933336903</v>
+        <v>2.1360139397911224</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.37034816399081855</v>
+        <v>0.36872120936504243</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.50736639109973303</v>
+        <v>0.50575891785357996</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.31531060905071073</v>
+        <v>0.31365851114517557</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.26281373970668764</v>
+        <v>0.26093017865784601</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.38057119548631552</v>
+        <v>0.37867133240150952</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.070759569989372384</v>
+        <v>0.068906038262757985</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.046033211013621962</v>
+        <v>0.044182055587727809</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.20270089841785699</v>
+        <v>0.20087840688674374</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.11897561412028082</v>
+        <v>0.11720761929005896</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.19407061377807575</v>
+        <v>0.19231661745942519</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.08824977518023476</v>
+        <v>0.086437977771908592</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.12066601873160429</v>
+        <v>0.11882932774353336</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.10100422563835698</v>
+        <v>0.099169656590752053</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.025613906251685872</v>
+        <v>0.023777124192886384</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.028506671130456532</v>
+        <v>0.026667292763101903</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.060528455389440031</v>
+        <v>0.05873889055617007</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.13823402758326933</v>
+        <v>0.13647181440632178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.043304350863425871</v>
+        <v>0.041508201464209332</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.12722955060033228</v>
+        <v>0.12547377449851252</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.053597248415727675</v>
+        <v>0.051774328763595973</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.05299562921300098</v>
+        <v>0.051176462020794011</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.024938012907093333</v>
+        <v>0.023111647399819371</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.024004944000241748</v>
+        <v>0.022175170233107087</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.039750824084963519</v>
+        <v>0.03792953825870151</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.029120817315459804</v>
+        <v>0.027297144788880987</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.027058039572493225</v>
+        <v>0.025236278779534403</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.028326209825181317</v>
+        <v>0.02649959749807251</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.032339192435661614</v>
+        <v>0.030518950516186621</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.029550812044400881</v>
+        <v>0.027731874171922563</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.026832987103716979</v>
+        <v>0.025014689404894343</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.028421623793692199</v>
+        <v>0.02660239922003271</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.02843394204162911</v>
+        <v>0.026611369521752328</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.02638535239174283</v>
+        <v>0.024557125901350126</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.037272808616460013</v>
+        <v>0.035456452384477581</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.030873981989528582</v>
+        <v>0.029053029017104062</v>
       </c>
     </row>
     <row r="38">

</xml_diff>

<commit_message>
varias generaciones de funciones para ahorrar espacio en el main, ademas de automatizar el nodo con dano a partir de un elemento tubular
</commit_message>
<xml_diff>
--- a/Resultados/P_18.xlsx
+++ b/Resultados/P_18.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" uniqueCount="1">
   <si>
     <t>P</t>
   </si>
@@ -67,7 +67,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="true"/>
+    <col min="1" max="1" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -77,182 +77,182 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>2.1360139397911224</v>
+        <v>0.60995931606694376</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.36872120936504243</v>
+        <v>0.83355497761059105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.50575891785357996</v>
+        <v>0.73250076650668305</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.31365851114517557</v>
+        <v>0.7165717039853946</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.26093017865784601</v>
+        <v>0.61984130807822369</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.37867133240150952</v>
+        <v>0.66931913000456766</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.068906038262757985</v>
+        <v>0.72186787213185144</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.044182055587727809</v>
+        <v>0.65183093080878007</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.20087840688674374</v>
+        <v>0.64675694385725657</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.11720761929005896</v>
+        <v>0.66252816554234628</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.19231661745942519</v>
+        <v>0.69000103550874581</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.086437977771908592</v>
+        <v>0.66309721044387027</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.11882932774353336</v>
+        <v>0.62459718320523083</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.099169656590752053</v>
+        <v>0.64702839335258366</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.023777124192886384</v>
+        <v>0.6550904217207415</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.026667292763101903</v>
+        <v>0.67643270861422555</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.05873889055617007</v>
+        <v>0.68753693218394185</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.13647181440632178</v>
+        <v>0.67552390375129034</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.041508201464209332</v>
+        <v>0.67240435903540374</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.12547377449851252</v>
+        <v>0.62937618625795244</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.051774328763595973</v>
+        <v>0.64890432386180164</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.051176462020794011</v>
+        <v>0.59441390974804431</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.023111647399819371</v>
+        <v>0.61656945535666285</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.022175170233107087</v>
+        <v>0.70441661544026879</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.03792953825870151</v>
+        <v>0.65352193853913143</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.027297144788880987</v>
+        <v>0.62280237368780889</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.025236278779534403</v>
+        <v>0.72343567692511934</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.02649959749807251</v>
+        <v>0.70057597564136309</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.030518950516186621</v>
+        <v>0.66098272492859622</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.027731874171922563</v>
+        <v>0.63271021164838903</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.025014689404894343</v>
+        <v>0.65393952664769461</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.02660239922003271</v>
+        <v>0.79501311532159047</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.026611369521752328</v>
+        <v>0.74672234775261737</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.024557125901350126</v>
+        <v>0.63240445833042613</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.035456452384477581</v>
+        <v>0.7167552527227784</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.029053029017104062</v>
+        <v>2.1071601324810114</v>
       </c>
     </row>
     <row r="38">

</xml_diff>